<commit_message>
Changes to login credentials
</commit_message>
<xml_diff>
--- a/Data Files/Login Data File/Login.xlsx
+++ b/Data Files/Login Data File/Login.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chweya\Katalon Studio\MKOPA LOGIN\Data Files\Login Data File\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lewis.mocha\git\MKOPA_Regression_Test_Channel\Data Files\Login Data File\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="993"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="993"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
   <si>
     <t>url</t>
   </si>
@@ -43,20 +43,23 @@
     <t>wrong</t>
   </si>
   <si>
-    <t>Chesangkip-1235</t>
-  </si>
-  <si>
     <t>pascal.kipkemoi@m-kopa.com</t>
   </si>
   <si>
     <t>Mkopa-12345</t>
+  </si>
+  <si>
+    <t>gideon.arita@m-kopa.com</t>
+  </si>
+  <si>
+    <t>Mikhitaryan16?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -85,6 +88,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -107,13 +116,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -398,18 +408,18 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.140625"/>
-    <col min="2" max="2" width="29.7109375"/>
-    <col min="3" max="3" width="16.7109375"/>
-    <col min="4" max="1025" width="8.5703125"/>
+    <col min="1" max="1" width="25.109375"/>
+    <col min="2" max="2" width="29.6640625"/>
+    <col min="3" max="3" width="16.6640625"/>
+    <col min="4" max="1025" width="8.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -420,12 +430,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -433,29 +443,29 @@
         <v>4</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="B5" s="6" t="s">
         <v>7</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -465,10 +475,9 @@
     <hyperlink ref="A4" r:id="rId3"/>
     <hyperlink ref="B4" r:id="rId4"/>
     <hyperlink ref="A5" r:id="rId5"/>
-    <hyperlink ref="B5" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
 
@@ -478,9 +487,9 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1025" width="8.5703125"/>
+    <col min="1" max="1025" width="8.5546875"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -494,9 +503,9 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1025" width="8.5703125"/>
+    <col min="1" max="1025" width="8.5546875"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>